<commit_message>
updated ui ux message sending templeted
</commit_message>
<xml_diff>
--- a/recipients.xlsx
+++ b/recipients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one\emailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D9EA8-2A4A-4810-98CF-9AB0B438A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22018EC-0964-44D6-95D4-F1AD4AF2BCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41210A71-C1B3-46AF-9E8F-39CF8A4928ED}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>Computer Science</t>
   </si>
   <si>
-    <t>your email</t>
+    <t>sender mail</t>
   </si>
 </sst>
 </file>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AC1604-2A15-43C7-B709-23A7B5BBAB66}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,10 +460,10 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="premkumar995252@gmail.com" xr:uid="{EC5404AD-40AE-475C-8CC1-920D2FDB5C83}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>